<commit_message>
Finish database format draft, add info to county jail summary
</commit_message>
<xml_diff>
--- a/docs/County-jail-summaries.xlsx
+++ b/docs/County-jail-summaries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
   <si>
     <t>County</t>
   </si>
@@ -168,9 +168,6 @@
     <t>https://www.whitfieldcountyga.com/p2c/jailinmates.aspx</t>
   </si>
   <si>
-    <t>Even if "Yes", release date may be</t>
-  </si>
-  <si>
     <t>inmates, depending on the county.</t>
   </si>
   <si>
@@ -190,13 +187,169 @@
   </si>
   <si>
     <t xml:space="preserve">spotty (ex: only posting releases for </t>
+  </si>
+  <si>
+    <t>When should booking expire?</t>
+  </si>
+  <si>
+    <t>Drop off roster</t>
+  </si>
+  <si>
+    <t>After 1 day</t>
+  </si>
+  <si>
+    <t>Drop off roster or current status changes to something that indicates they had a trial</t>
+  </si>
+  <si>
+    <t>Current day's arrests &amp; releases posted, but that's all we can get.</t>
+  </si>
+  <si>
+    <t>Infinite</t>
+  </si>
+  <si>
+    <t>Releases posted for bookings &lt;=7 days ago. For &gt;7 days, see when they dropped off roster or current status changes to something like "sentenced" indicating they had a trial</t>
+  </si>
+  <si>
+    <t>Impossible</t>
+  </si>
+  <si>
+    <t>After 72 hours</t>
+  </si>
+  <si>
+    <t>After 30 days</t>
+  </si>
+  <si>
+    <t>How to get "total days jailed pre-trial"</t>
+  </si>
+  <si>
+    <t>When listed as released</t>
+  </si>
+  <si>
+    <t>When listed as released or current status changes to something that indicates they had a trial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">current status like 'Sentenced' but maybe we can assume </t>
+  </si>
+  <si>
+    <t>Biggest # days we can get for "at least X days jailed before release"</t>
+  </si>
+  <si>
+    <t>See when they dropped off roster</t>
+  </si>
+  <si>
+    <t>See when they dropped off roster or current status changes to something like "sentenced" indicating they had a trial</t>
+  </si>
+  <si>
+    <t>If all we know is they dropped off roster, we don't know if they were released pre-trial or other reason, like sentenced or transferred to state prison!</t>
+  </si>
+  <si>
+    <t>Can get bookings &amp; releases on any date (not all releases are pre-trial). See when current status changes to something like "sentenced" indicating they had a trial</t>
+  </si>
+  <si>
+    <t>Can get bookings &amp; releases on any date (not all releases are pre-trial). Can't see whether they had a trial or not</t>
+  </si>
+  <si>
+    <t>Releases posted for bookings &lt;=30 days ago or current status changes to something like "sentenced" indicating they had a trial.</t>
+  </si>
+  <si>
+    <t>See when they dropped off roster or current status changes to something like "sentenced" indicating they had a trial.</t>
+  </si>
+  <si>
+    <t>When listed as released, drop off roster or current status changes to something that indicates they had a trial</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">See when they dropped off roster or when court date occurs indicating they had a trial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Unless that’s the arraignment - not sure what court date means)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drop off roster or after court date occurs indicating they had a trial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Unless that’s the arraignment - not sure what court date means)</t>
+    </r>
+  </si>
+  <si>
+    <t>Releases posted for last 14 days (not all releases are pre-trial)</t>
+  </si>
+  <si>
+    <t>someone released after &lt;7 days is probably pre-trial?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">See when they dropped off roster or current status changes to something like "sentenced" indicating they had a trial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(confused, if it only lists current inmates why are some dispositions 'released'?)</t>
+    </r>
+  </si>
+  <si>
+    <t>Infinite (but only see drop off roster)</t>
+  </si>
+  <si>
+    <t>7 (for &gt;7 days, only see drop off roster)</t>
+  </si>
+  <si>
+    <t>For some counties we can figure out if release was pretrial using bond info &amp;</t>
+  </si>
+  <si>
+    <r>
+      <t>Drop off ro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ster or current status changes to something that indicates they had a trial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(confused, if it only lists current inmates why are some dispositions 'released'?)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +378,27 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -287,6 +461,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,10 +781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,14 +793,15 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="180.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="100.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,22 +812,31 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -651,19 +847,28 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -679,11 +884,20 @@
       <c r="E3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -694,22 +908,31 @@
         <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -725,11 +948,20 @@
       <c r="E5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="16">
+        <v>30</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -745,11 +977,20 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -765,11 +1006,20 @@
       <c r="E7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -785,11 +1035,20 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,11 +1064,20 @@
       <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -825,14 +1093,23 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -848,14 +1125,23 @@
       <c r="E11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -871,11 +1157,20 @@
       <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -886,16 +1181,25 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -911,11 +1215,20 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -931,11 +1244,20 @@
       <c r="E15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -946,16 +1268,25 @@
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -971,11 +1302,20 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -989,74 +1329,88 @@
       </c>
       <c r="D19" s="4">
         <f>COUNTIF(D2:D17,"Yes")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4">
         <f>COUNTIF(E2:E17,"Yes")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="D20" s="11" t="s">
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="G4" r:id="rId4"/>
-    <hyperlink ref="F3" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="F5" r:id="rId7"/>
-    <hyperlink ref="F6" r:id="rId8"/>
-    <hyperlink ref="F7" r:id="rId9" location="/search" display="https://ody.dekalbcountyga.gov/app/JailSearch/ - /search"/>
-    <hyperlink ref="F8" r:id="rId10"/>
-    <hyperlink ref="F9" r:id="rId11"/>
-    <hyperlink ref="F10" r:id="rId12"/>
-    <hyperlink ref="G10" r:id="rId13"/>
-    <hyperlink ref="G11" r:id="rId14" display="https://performance.fultoncountyga.gov/stories/s/Jail-Report/ts5s-mgr9/"/>
-    <hyperlink ref="F11" r:id="rId15"/>
-    <hyperlink ref="F12" r:id="rId16"/>
-    <hyperlink ref="F13" r:id="rId17"/>
-    <hyperlink ref="F14" r:id="rId18" display="http://www.lowndessheriff.com/default.asp?P=current_inmates"/>
-    <hyperlink ref="F15" r:id="rId19"/>
-    <hyperlink ref="F16" r:id="rId20"/>
-    <hyperlink ref="F17" r:id="rId21"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="J4" r:id="rId4"/>
+    <hyperlink ref="I3" r:id="rId5"/>
+    <hyperlink ref="K4" r:id="rId6"/>
+    <hyperlink ref="I5" r:id="rId7"/>
+    <hyperlink ref="I6" r:id="rId8"/>
+    <hyperlink ref="I7" r:id="rId9" location="/search" display="https://ody.dekalbcountyga.gov/app/JailSearch/ - /search"/>
+    <hyperlink ref="I8" r:id="rId10"/>
+    <hyperlink ref="I9" r:id="rId11"/>
+    <hyperlink ref="I10" r:id="rId12"/>
+    <hyperlink ref="J10" r:id="rId13"/>
+    <hyperlink ref="J11" r:id="rId14" display="https://performance.fultoncountyga.gov/stories/s/Jail-Report/ts5s-mgr9/"/>
+    <hyperlink ref="I11" r:id="rId15"/>
+    <hyperlink ref="I12" r:id="rId16"/>
+    <hyperlink ref="I13" r:id="rId17"/>
+    <hyperlink ref="I14" r:id="rId18" display="http://www.lowndessheriff.com/default.asp?P=current_inmates"/>
+    <hyperlink ref="I15" r:id="rId19"/>
+    <hyperlink ref="I16" r:id="rId20"/>
+    <hyperlink ref="I17" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId22"/>

</xml_diff>

<commit_message>
Add known felonies to minimal database
</commit_message>
<xml_diff>
--- a/docs/County-jail-summaries.xlsx
+++ b/docs/County-jail-summaries.xlsx
@@ -447,11 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -469,8 +465,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -785,7 +785,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F6" sqref="F6"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
       <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -836,128 +836,128 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="14">
         <v>1</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="16">
         <v>1</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="14">
         <v>30</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -977,45 +977,45 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1035,45 +1035,45 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="12" t="s">
         <v>59</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1109,35 +1109,35 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1228,32 +1228,32 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1302,13 +1302,13 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>59</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -1335,10 +1335,10 @@
         <f>COUNTIF(E2:E17,"Yes")</f>
         <v>10</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1347,38 +1347,38 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="13"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="11" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change ETL to make timestamps that have only date be set to noon
</commit_message>
<xml_diff>
--- a/docs/County-jail-summaries.xlsx
+++ b/docs/County-jail-summaries.xlsx
@@ -785,7 +785,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F3" sqref="F3"/>
+      <selection pane="topRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,95 +1050,95 @@
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1400,11 +1400,11 @@
     <hyperlink ref="I6" r:id="rId8"/>
     <hyperlink ref="I7" r:id="rId9" location="/search" display="https://ody.dekalbcountyga.gov/app/JailSearch/ - /search"/>
     <hyperlink ref="I8" r:id="rId10"/>
-    <hyperlink ref="I9" r:id="rId11"/>
-    <hyperlink ref="I10" r:id="rId12"/>
-    <hyperlink ref="J10" r:id="rId13"/>
-    <hyperlink ref="J11" r:id="rId14" display="https://performance.fultoncountyga.gov/stories/s/Jail-Report/ts5s-mgr9/"/>
-    <hyperlink ref="I11" r:id="rId15"/>
+    <hyperlink ref="I10" r:id="rId11"/>
+    <hyperlink ref="I11" r:id="rId12"/>
+    <hyperlink ref="J11" r:id="rId13"/>
+    <hyperlink ref="J9" r:id="rId14" display="https://performance.fultoncountyga.gov/stories/s/Jail-Report/ts5s-mgr9/"/>
+    <hyperlink ref="I9" r:id="rId15"/>
     <hyperlink ref="I12" r:id="rId16"/>
     <hyperlink ref="I13" r:id="rId17"/>
     <hyperlink ref="I14" r:id="rId18" display="http://www.lowndessheriff.com/default.asp?P=current_inmates"/>

</xml_diff>